<commit_message>
top cover (one half) and LIDAR added
</commit_message>
<xml_diff>
--- a/RUR-2_testing og assem2/BOM.xlsx
+++ b/RUR-2_testing og assem2/BOM.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8422152E-367F-0841-815D-EFD5B23D9010}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="101" documentId="8_{8422152E-367F-0841-815D-EFD5B23D9010}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{FF96B6C7-A4E1-4323-9148-07B8109B9BEE}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11850" yWindow="3180" windowWidth="43200" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,6 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -29,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="42">
   <si>
     <t>Name</t>
   </si>
@@ -61,9 +60,6 @@
     <t>Total</t>
   </si>
   <si>
-    <t>Total MOQ</t>
-  </si>
-  <si>
     <t>Ø3,5mm x 20mm countersunk self-tapping screw</t>
   </si>
   <si>
@@ -113,6 +109,51 @@
   </si>
   <si>
     <t>M5 washer (locking)</t>
+  </si>
+  <si>
+    <t>Support wheels Penn-Elcomm-W0998</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RPLIDAR A1M8 - 360 DEGREE LASER </t>
+  </si>
+  <si>
+    <t>Incl</t>
+  </si>
+  <si>
+    <t>Bat pack</t>
+  </si>
+  <si>
+    <t>Jetson</t>
+  </si>
+  <si>
+    <t>M12 threaded rod</t>
+  </si>
+  <si>
+    <t>M5 threaded rod</t>
+  </si>
+  <si>
+    <t>M12 washers</t>
+  </si>
+  <si>
+    <t>Digikey</t>
+  </si>
+  <si>
+    <t>Penn-Elcomm</t>
+  </si>
+  <si>
+    <t>T5 timing belt 500mm</t>
+  </si>
+  <si>
+    <t>RS Ball bearing ID:12mm OD:28mm W:8mm</t>
+  </si>
+  <si>
+    <t>MOQ or QTY</t>
+  </si>
+  <si>
+    <t>Purchase sum</t>
+  </si>
+  <si>
+    <t>MOQ sum</t>
   </si>
 </sst>
 </file>
@@ -208,14 +249,14 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>56029</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>119415</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>114298</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>114297</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>137133</xdr:rowOff>
     </xdr:to>
@@ -533,20 +574,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B4:O15"/>
+  <dimension ref="B4:R29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="P23" sqref="P23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="45.87109375" customWidth="1"/>
-    <col min="4" max="7" width="9.14453125" style="1"/>
-    <col min="15" max="15" width="43.1796875" customWidth="1"/>
+    <col min="2" max="2" width="45.85546875" customWidth="1"/>
+    <col min="4" max="6" width="9.140625" style="1"/>
+    <col min="7" max="7" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" style="1"/>
+    <col min="9" max="9" width="0" style="1" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="15" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="43.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>0</v>
       </c>
@@ -563,27 +609,36 @@
         <v>8</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H4" t="s">
+        <v>41</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="K4" t="s">
         <v>3</v>
       </c>
-      <c r="I4" t="s">
+      <c r="L4" t="s">
         <v>5</v>
       </c>
-      <c r="J4" t="s">
+      <c r="M4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C5" s="2">
         <v>60</v>
       </c>
-      <c r="D5" s="3">
-        <f>G5/F5</f>
+      <c r="D5" s="1">
+        <f t="shared" ref="D5:D7" si="0">IFERROR(G5/F5,0)</f>
         <v>0.41509999999999997</v>
       </c>
       <c r="E5" s="3">
@@ -596,26 +651,37 @@
       <c r="G5" s="3">
         <v>41.51</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="H5" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="I5" s="3" t="b">
+        <f>IF(E5&gt;G5,TRUE,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="J5" s="1">
+        <f t="shared" ref="J5:J23" si="1">IF(H5,IF(I5,E5,G5),0)</f>
+        <v>0</v>
+      </c>
+      <c r="K5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="I5" s="2">
+      <c r="L5" s="2">
         <v>2474985</v>
       </c>
-      <c r="J5" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="M5" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C6">
         <f>3*4+8*6</f>
         <v>60</v>
       </c>
       <c r="D6" s="1">
-        <f>G6/F6</f>
+        <f t="shared" si="0"/>
         <v>0.46500000000000002</v>
       </c>
       <c r="E6" s="1">
@@ -628,25 +694,36 @@
       <c r="G6" s="1">
         <v>46.5</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="I6" s="1" t="b">
+        <f t="shared" ref="I6:I27" si="2">IF(E6&gt;G6,TRUE,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="J6" s="1">
+        <f t="shared" si="1"/>
+        <v>46.5</v>
+      </c>
+      <c r="K6" t="s">
         <v>4</v>
       </c>
-      <c r="I6">
+      <c r="L6">
         <v>2475006</v>
       </c>
-      <c r="J6" s="4" t="s">
+      <c r="M6" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B7" t="s">
-        <v>13</v>
       </c>
       <c r="C7">
         <v>2</v>
       </c>
       <c r="D7" s="1">
-        <f>G7/F7</f>
+        <f t="shared" si="0"/>
         <v>0.78369999999999995</v>
       </c>
       <c r="E7" s="1">
@@ -659,93 +736,608 @@
       <c r="G7">
         <v>7.8369999999999997</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H7" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="I7" s="1" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J7" s="1">
+        <f t="shared" si="1"/>
+        <v>7.8369999999999997</v>
+      </c>
+      <c r="K7" t="s">
+        <v>13</v>
+      </c>
+      <c r="L7" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="I7" s="4" t="s">
+      <c r="M7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="N7" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="J7" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="K7" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="N7" s="4"/>
-      <c r="O7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="2:15" ht="27.75" x14ac:dyDescent="0.2">
+      <c r="Q7" s="4"/>
+      <c r="R7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="2:18" ht="30" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C8">
         <v>2</v>
       </c>
-      <c r="K8" t="s">
-        <v>17</v>
-      </c>
-      <c r="O8" s="5" t="s">
+      <c r="D8" s="1">
+        <f>IFERROR(G8/F8,0)</f>
+        <v>0</v>
+      </c>
+      <c r="E8" s="1">
+        <f t="shared" ref="E8:E18" si="3">D8*C8</f>
+        <v>0</v>
+      </c>
+      <c r="H8" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="I8" s="1" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J8" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N8" t="s">
+        <v>16</v>
+      </c>
+      <c r="R8" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B9" t="s">
+      <c r="D9" s="1">
+        <f t="shared" ref="D9:D19" si="4">IFERROR(G9/F9,0)</f>
+        <v>0</v>
+      </c>
+      <c r="E9" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="H9" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="I9" s="1" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J9" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B10" t="s">
-        <v>22</v>
       </c>
       <c r="C10">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="D10" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="E10" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="H10" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="I10" s="1" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J10" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11" s="1">
+        <f t="shared" ref="D11" si="5">IFERROR(G11/F11,0)</f>
+        <v>0</v>
+      </c>
+      <c r="E11" s="1">
+        <f t="shared" ref="E11" si="6">D11*C11</f>
+        <v>0</v>
+      </c>
+      <c r="H11" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="I11" s="1" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J11" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
+      <c r="D12" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="E12" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="H12" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="I12" s="1" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J12" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13">
+        <v>2</v>
+      </c>
+      <c r="D13" s="1">
+        <f t="shared" ref="D13" si="7">IFERROR(G13/F13,0)</f>
+        <v>0</v>
+      </c>
+      <c r="E13" s="1">
+        <f t="shared" ref="E13" si="8">D13*C13</f>
+        <v>0</v>
+      </c>
+      <c r="H13" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="I13" s="1" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J13" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="E14" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="H14" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="I14" s="1" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J14" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
         <v>23</v>
       </c>
-      <c r="C11">
+      <c r="C15">
+        <v>4</v>
+      </c>
+      <c r="D15" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="E15" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="H15" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="I15" s="1" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J15" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16">
+        <v>6</v>
+      </c>
+      <c r="D16" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="E16" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="H16" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="I16" s="1" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J16" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>25</v>
+      </c>
+      <c r="D17" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="E17" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="H17" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="I17" s="1" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J17" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>26</v>
+      </c>
+      <c r="D18" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="E18" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="H18" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="I18" s="1" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J18" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19">
         <v>2</v>
       </c>
-    </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B12" t="s">
-        <v>24</v>
-      </c>
-      <c r="C12">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B13" t="s">
-        <v>25</v>
-      </c>
-      <c r="C13">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B14" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="15" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B15" t="s">
-        <v>27</v>
+      <c r="D19" s="1">
+        <f t="shared" si="4"/>
+        <v>29.3</v>
+      </c>
+      <c r="E19" s="1">
+        <f>D19*C19</f>
+        <v>58.6</v>
+      </c>
+      <c r="F19" s="1">
+        <v>1</v>
+      </c>
+      <c r="G19" s="1">
+        <v>29.3</v>
+      </c>
+      <c r="H19" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="I19" s="1" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="J19" s="1">
+        <f t="shared" si="1"/>
+        <v>58.6</v>
+      </c>
+      <c r="K19" t="s">
+        <v>36</v>
+      </c>
+      <c r="M19" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20" s="1">
+        <f t="shared" ref="D20" si="9">IFERROR(G20/F20,0)</f>
+        <v>610</v>
+      </c>
+      <c r="E20" s="1">
+        <f>D20*C20</f>
+        <v>610</v>
+      </c>
+      <c r="F20" s="1">
+        <v>1</v>
+      </c>
+      <c r="G20" s="1">
+        <v>610</v>
+      </c>
+      <c r="H20" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="I20" s="1" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J20" s="1">
+        <f t="shared" si="1"/>
+        <v>610</v>
+      </c>
+      <c r="K20" t="s">
+        <v>35</v>
+      </c>
+      <c r="M20" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>30</v>
+      </c>
+      <c r="D21" s="1">
+        <f t="shared" ref="D21:D27" si="10">IFERROR(G21/F21,0)</f>
+        <v>0</v>
+      </c>
+      <c r="E21" s="1">
+        <f t="shared" ref="E21:E27" si="11">D21*C21</f>
+        <v>0</v>
+      </c>
+      <c r="H21" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="I21" s="1" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J21" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>31</v>
+      </c>
+      <c r="D22" s="1">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="E22" s="1">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="H22" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="I22" s="1" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J22" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>37</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23" s="1">
+        <f t="shared" si="10"/>
+        <v>65.78</v>
+      </c>
+      <c r="E23" s="1">
+        <f t="shared" si="11"/>
+        <v>65.78</v>
+      </c>
+      <c r="F23" s="1">
+        <v>1</v>
+      </c>
+      <c r="G23" s="1">
+        <v>65.78</v>
+      </c>
+      <c r="H23" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="I23" s="1" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J23" s="1">
+        <f t="shared" si="1"/>
+        <v>65.78</v>
+      </c>
+      <c r="M23" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>38</v>
+      </c>
+      <c r="C24">
+        <v>2</v>
+      </c>
+      <c r="D24" s="1">
+        <f t="shared" si="10"/>
+        <v>23.85</v>
+      </c>
+      <c r="E24" s="1">
+        <f t="shared" si="11"/>
+        <v>47.7</v>
+      </c>
+      <c r="F24" s="1">
+        <v>1</v>
+      </c>
+      <c r="G24" s="1">
+        <v>23.85</v>
+      </c>
+      <c r="H24" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="I24" s="1" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="J24" s="1">
+        <f>IF(H24,IF(I24,E24,G24),0)</f>
+        <v>47.7</v>
+      </c>
+      <c r="M24" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="D25" s="1">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="E25" s="1">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="H25" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="I25" s="1" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J25" s="1">
+        <f t="shared" ref="J25:J27" si="12">IF(H25,IF(I25,E25,G25),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="D26" s="1">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="E26" s="1">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="H26" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="I26" s="1" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J26" s="1">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="D27" s="1">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="E27" s="1">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="H27" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="I27" s="1" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J27" s="1">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="J29" s="1">
+        <f>SUM(J5:J28)</f>
+        <v>836.41700000000003</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="J6" r:id="rId1" xr:uid="{5DA118E4-E553-44EB-8BF5-6FC6BEA68CC8}"/>
-    <hyperlink ref="J5" r:id="rId2" xr:uid="{B94274F9-3F5B-45B6-9083-BDBDF11699F2}"/>
-    <hyperlink ref="I7" r:id="rId3" tooltip="RS PRO Trykfjeder, 36mm x Ø5.8mm, 1.8N/mm" display="https://dk.rs-online.com/web/p/trykfjedre/0751534/" xr:uid="{63BF1319-4088-4DBF-AF59-F9B6B251695D}"/>
-    <hyperlink ref="J7" r:id="rId4" xr:uid="{2513CD69-2E1D-4FA8-A6D5-C7A98AF875D9}"/>
-    <hyperlink ref="K7" r:id="rId5" xr:uid="{A0FC88ED-5B7E-4138-A89C-9BF72F0D15E2}"/>
+    <hyperlink ref="M6" r:id="rId1" xr:uid="{5DA118E4-E553-44EB-8BF5-6FC6BEA68CC8}"/>
+    <hyperlink ref="M5" r:id="rId2" xr:uid="{B94274F9-3F5B-45B6-9083-BDBDF11699F2}"/>
+    <hyperlink ref="L7" r:id="rId3" tooltip="RS PRO Trykfjeder, 36mm x Ø5.8mm, 1.8N/mm" display="https://dk.rs-online.com/web/p/trykfjedre/0751534/" xr:uid="{63BF1319-4088-4DBF-AF59-F9B6B251695D}"/>
+    <hyperlink ref="M7" r:id="rId4" xr:uid="{2513CD69-2E1D-4FA8-A6D5-C7A98AF875D9}"/>
+    <hyperlink ref="N7" r:id="rId5" xr:uid="{A0FC88ED-5B7E-4138-A89C-9BF72F0D15E2}"/>
+    <hyperlink ref="M19" r:id="rId6" xr:uid="{18DF1E98-C8D8-4704-8B59-5174356DF90D}"/>
+    <hyperlink ref="M20" r:id="rId7" xr:uid="{4A47E5A2-6E19-42C3-A84A-5820C8A1B034}"/>
+    <hyperlink ref="M23" r:id="rId8" xr:uid="{59E2AE45-A166-4E52-9F45-244004CE8305}"/>
+    <hyperlink ref="M24" r:id="rId9" xr:uid="{E21978C5-77AD-459A-8781-BC46D4DDA488}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId6"/>
+  <drawing r:id="rId10"/>
 </worksheet>
 </file>
</xml_diff>